<commit_message>
Adding more classes and activities
</commit_message>
<xml_diff>
--- a/Organizacion/Horario_Semestre_1.xlsx
+++ b/Organizacion/Horario_Semestre_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuel.pasieka/Documents/projects/UNIR-IA/Organizacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A97BB4-D8F4-DD44-9536-6D8FDC6396E6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E01E422-5261-214B-9245-7303DB18A6CC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="32740" windowHeight="20540" xr2:uid="{74444228-8826-9247-9EB0-EE938561BEE4}"/>
+    <workbookView xWindow="880" yWindow="460" windowWidth="32720" windowHeight="20540" xr2:uid="{74444228-8826-9247-9EB0-EE938561BEE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -143,7 +143,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -190,6 +190,19 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color theme="1"/>
       </left>
       <right style="thin">
@@ -236,283 +249,307 @@
         <color theme="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color theme="1"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color theme="1"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color theme="1"/>
-      </right>
-      <top style="medium">
-        <color theme="1"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
+      </top>
+      <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="medium">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="medium">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -523,7 +560,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -544,22 +581,19 @@
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
@@ -642,6 +676,20 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="29" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -964,7 +1012,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1000,65 +1048,65 @@
       <c r="A2" s="3">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="18"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>0.375</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="E3" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="34" t="s">
-        <v>7</v>
-      </c>
+      <c r="F3" s="40"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="19"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
+      <c r="F4" s="33" t="s">
+        <v>7</v>
+      </c>
       <c r="G4" s="6"/>
-      <c r="H4" s="19"/>
+      <c r="H4" s="18"/>
     </row>
     <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>7.4583333333333304</v>
       </c>
-      <c r="B5" s="20"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="19"/>
+      <c r="H5" s="18"/>
     </row>
     <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>6.5</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="11"/>
@@ -1066,139 +1114,139 @@
         <v>8</v>
       </c>
       <c r="E6" s="11"/>
-      <c r="F6" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="19"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="18"/>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>5.5416666666666599</v>
       </c>
-      <c r="B7" s="22"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="11"/>
       <c r="D7" s="9"/>
       <c r="E7" s="11"/>
-      <c r="F7" s="9"/>
+      <c r="F7" s="43" t="s">
+        <v>8</v>
+      </c>
       <c r="G7" s="6"/>
-      <c r="H7" s="19"/>
+      <c r="H7" s="18"/>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>4.5833333333333304</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="36" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="31"/>
-      <c r="E8" s="36" t="s">
+      <c r="D8" s="30"/>
+      <c r="E8" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="9"/>
+      <c r="F8" s="44"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="19"/>
+      <c r="H8" s="18"/>
     </row>
     <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>3.625</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="13"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="44"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="19"/>
+      <c r="H9" s="18"/>
     </row>
     <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>2.6666666666666599</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="37" t="s">
+      <c r="C10" s="13"/>
+      <c r="D10" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="37" t="s">
-        <v>9</v>
-      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="45"/>
       <c r="G10" s="12"/>
-      <c r="H10" s="19"/>
+      <c r="H10" s="18"/>
     </row>
     <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>1.7083333333333299</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="G11" s="12"/>
-      <c r="H11" s="19"/>
+      <c r="H11" s="18"/>
     </row>
     <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>0.74999999999998901</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
       <c r="G12" s="12"/>
-      <c r="H12" s="19"/>
+      <c r="H12" s="18"/>
     </row>
     <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>0.79166666666666097</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="37" t="s">
+      <c r="C13" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
       <c r="G13" s="12"/>
-      <c r="H13" s="19"/>
+      <c r="H13" s="18"/>
     </row>
     <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>0.83333333333329995</v>
       </c>
-      <c r="B14" s="39"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="37" t="s">
+      <c r="B14" s="38"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="37" t="s">
+      <c r="F14" s="36" t="s">
         <v>10</v>
       </c>
       <c r="G14" s="12"/>
-      <c r="H14" s="19"/>
+      <c r="H14" s="18"/>
     </row>
     <row r="15" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>0.875</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="27"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="26"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
@@ -1219,7 +1267,7 @@
   <mergeCells count="3">
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="D6:D9"/>
-    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="F7:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>